<commit_message>
running database mapping qmd
</commit_message>
<xml_diff>
--- a/mapping_final/matched_partial_tmp.xlsx
+++ b/mapping_final/matched_partial_tmp.xlsx
@@ -15984,13 +15984,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A5FC6A-5A35-419B-A610-FEEF8175ADD4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A8DBCC6-8C46-4E97-9450-EE063997DE0D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{509C45C4-F508-42CD-8C46-A91218F0D21C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D86E61-B289-4EDF-93A4-00E11ECEAFD7}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D37F5124-F39B-4855-9985-319674C793F7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A07EFBD-9488-4BFF-9DA2-5E5E399B9FDD}"/>
 </file>
</xml_diff>